<commit_message>
Add createHit without HitTypeId, tests & impl
</commit_message>
<xml_diff>
--- a/Modulos, Entidades, Operaciones y Prioridades.xlsx
+++ b/Modulos, Entidades, Operaciones y Prioridades.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Saldos Iniciales" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="63">
   <si>
     <t>ApproveAssignment</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>SEARCH</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -214,6 +220,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,34 +315,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="29">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -362,18 +369,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D42" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E42" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E42"/>
   <sortState ref="A2:D42">
     <sortCondition ref="C2:C42"/>
     <sortCondition ref="B2:B42"/>
     <sortCondition ref="D2:D42"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" name="Operation"/>
     <tableColumn id="2" name="Main Related Entity"/>
     <tableColumn id="3" name="Module"/>
     <tableColumn id="4" name="OperationType (READ/WRITE/SEARCH)"/>
+    <tableColumn id="5" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -714,7 +722,7 @@
     <col min="4" max="4" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -727,8 +735,11 @@
       <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -742,7 +753,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -756,7 +767,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -770,7 +781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -784,7 +795,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -798,7 +809,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -812,7 +823,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -825,8 +836,11 @@
       <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -840,7 +854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -854,7 +868,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -868,7 +882,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -882,7 +896,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -896,7 +910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -910,7 +924,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -924,7 +938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -938,7 +952,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -952,7 +966,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -965,8 +979,11 @@
       <c r="D18" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -980,7 +997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -994,7 +1011,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1008,7 +1025,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1022,7 +1039,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1036,7 +1053,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1067,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1064,7 +1081,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1078,7 +1095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1092,7 +1109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1106,7 +1123,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1120,7 +1137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1134,7 +1151,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -1147,8 +1164,11 @@
       <c r="D31" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Complex create hit operation with registered hit type test implemented
</commit_message>
<xml_diff>
--- a/Modulos, Entidades, Operaciones y Prioridades.xlsx
+++ b/Modulos, Entidades, Operaciones y Prioridades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Saldos Iniciales" sheetId="2" r:id="rId1"/>
@@ -712,7 +712,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
remove useless hit layout domain
</commit_message>
<xml_diff>
--- a/Modulos, Entidades, Operaciones y Prioridades.xlsx
+++ b/Modulos, Entidades, Operaciones y Prioridades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
   <si>
     <t>ApproveAssignment</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Column1</t>
+  </si>
+  <si>
+    <t>Falta Layouts</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -369,19 +375,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:E42" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F42" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F42"/>
   <sortState ref="A2:D42">
     <sortCondition ref="C2:C42"/>
     <sortCondition ref="B2:B42"/>
     <sortCondition ref="D2:D42"/>
   </sortState>
-  <tableColumns count="5">
+  <tableColumns count="6">
     <tableColumn id="1" name="Operation"/>
     <tableColumn id="2" name="Main Related Entity"/>
     <tableColumn id="3" name="Module"/>
     <tableColumn id="4" name="OperationType (READ/WRITE/SEARCH)"/>
     <tableColumn id="5" name="Column1"/>
+    <tableColumn id="6" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -722,7 +729,7 @@
     <col min="4" max="4" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -738,8 +745,11 @@
       <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -753,7 +763,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -767,7 +777,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -781,7 +791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -795,7 +805,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -809,7 +819,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -823,7 +833,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -839,8 +849,11 @@
       <c r="E8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -854,7 +867,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -868,7 +881,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -882,7 +895,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -896,7 +909,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -910,7 +923,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -924,7 +937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -938,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Intermediate Grant qualifications commit
</commit_message>
<xml_diff>
--- a/Modulos, Entidades, Operaciones y Prioridades.xlsx
+++ b/Modulos, Entidades, Operaciones y Prioridades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
   <si>
     <t>ApproveAssignment</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>Column2</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
+  </si>
+  <si>
+    <t>REQUIRES Qualification Request entity creation</t>
   </si>
 </sst>
 </file>
@@ -283,8 +289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -335,6 +347,9 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -349,6 +364,9 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -719,7 +737,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -965,7 +983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -979,7 +997,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -996,7 +1014,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1010,7 +1028,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1024,7 +1042,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1038,7 +1056,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1051,8 +1069,11 @@
       <c r="D22" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1065,8 +1086,14 @@
       <c r="D23" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1080,7 +1107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1094,7 +1121,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1122,7 +1149,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1136,7 +1163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1150,7 +1177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1164,7 +1191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1208,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
GrantQualification implemntation and tests added
</commit_message>
<xml_diff>
--- a/Modulos, Entidades, Operaciones y Prioridades.xlsx
+++ b/Modulos, Entidades, Operaciones y Prioridades.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t>ApproveAssignment</t>
   </si>
@@ -214,12 +214,6 @@
   </si>
   <si>
     <t>Column2</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
-    <t>REQUIRES Qualification Request entity creation</t>
   </si>
 </sst>
 </file>
@@ -983,7 +977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -997,7 +991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1014,7 +1008,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1028,7 +1022,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1042,7 +1036,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1056,7 +1050,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1073,7 +1067,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1087,13 +1081,10 @@
         <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1121,7 +1112,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1126,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1149,7 +1140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1163,7 +1154,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1177,7 +1168,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1182,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>36</v>
       </c>

</xml_diff>